<commit_message>
Change name of untitled file to pydriller_test
</commit_message>
<xml_diff>
--- a/Sprint_1/repos/results/results.xlsx
+++ b/Sprint_1/repos/results/results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ML_exercises\CS7CS5-202122-Dissertation\Sprint_1\repos\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE41D9A-8519-4ED3-9487-0EDB1A99F0F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBD93BF-9F20-4A00-A123-3C4A2F19EC4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{52F7B8C6-ED79-4422-B4E2-3C12B17FB23E}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregated" sheetId="1" r:id="rId1"/>
-    <sheet name="Per-Month" sheetId="2" r:id="rId2"/>
-    <sheet name="Per-Author" sheetId="3" r:id="rId3"/>
+    <sheet name="By-Month" sheetId="2" r:id="rId2"/>
+    <sheet name="By-Author" sheetId="3" r:id="rId3"/>
     <sheet name="Terms" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
@@ -988,6 +988,290 @@
   </cellStyles>
   <dxfs count="87">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1016,6 +1300,370 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1199,654 +1847,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2449,21 +2449,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C0C797F-5A79-4F40-B092-BB00BE5C2C7F}" name="Month_Table" displayName="Month_Table" ref="A1:J121" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C0C797F-5A79-4F40-B092-BB00BE5C2C7F}" name="Month_Table" displayName="Month_Table" ref="A1:J121" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="A1:J121" xr:uid="{01ABD37D-F83F-4642-BFDB-B92B9C30E5A4}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D01A52EA-F873-41A8-AF9B-24DCF719E4AA}" name="Repository Rank" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{339B1CCD-C64A-45BD-97C4-539A8C29A379}" name="Repository Name" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{DF40CB11-7EAE-4B4B-8526-1E187C34811B}" name="Marker" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{2F18F556-AB38-494E-A097-F01F0F98393D}" name="Trend in Mean" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{A67A06C9-CBF0-4737-AC70-3591231E2765}" name="Month Eq (pre)" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{4AF80F60-D4BF-4B80-886D-FA3D7B97FF7F}" name="Month Eq (post)" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{E0E50CCA-870A-4D82-8F79-4423AD68F464}" name="Change Direction_x000a_(Month Eq)" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{D01A52EA-F873-41A8-AF9B-24DCF719E4AA}" name="Repository Rank" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{339B1CCD-C64A-45BD-97C4-539A8C29A379}" name="Repository Name" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{DF40CB11-7EAE-4B4B-8526-1E187C34811B}" name="Marker" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{2F18F556-AB38-494E-A097-F01F0F98393D}" name="Trend in Mean" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{A67A06C9-CBF0-4737-AC70-3591231E2765}" name="Month Eq (pre)" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{4AF80F60-D4BF-4B80-886D-FA3D7B97FF7F}" name="Month Eq (post)" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{E0E50CCA-870A-4D82-8F79-4423AD68F464}" name="Change Direction_x000a_(Month Eq)" dataDxfId="34">
       <calculatedColumnFormula>IF(Month_Table[Month Eq (pre)] &lt; Month_Table[Month Eq (post)], "Up", IF(Month_Table[Month Eq (pre)] &gt; Month_Table[Month Eq (post)], "Down", "No Change"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FFA93A9C-7A33-4017-9B34-5194BEA2CFB3}" name="Month 80 (pre)" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{5A3D6698-1492-42F4-9406-1B2DCCDA7B98}" name="Month 80 (post)" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{E8B4CBBA-F989-4D44-94D1-F8F9ED5AF158}" name="Change Direction_x000a_(Month 80)" dataDxfId="49">
+    <tableColumn id="5" xr3:uid="{FFA93A9C-7A33-4017-9B34-5194BEA2CFB3}" name="Month 80 (pre)" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{5A3D6698-1492-42F4-9406-1B2DCCDA7B98}" name="Month 80 (post)" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{E8B4CBBA-F989-4D44-94D1-F8F9ED5AF158}" name="Change Direction_x000a_(Month 80)" dataDxfId="31">
       <calculatedColumnFormula>IF(Month_Table[Month 80 (pre)] &lt; Month_Table[Month 80 (post)], "Up", IF(Month_Table[Month 80 (pre)] &gt; Month_Table[Month 80 (post)], "Down", "No Change"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2472,21 +2472,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D4467437-2A3E-4C21-932F-B15782EE29D5}" name="Author_Table" displayName="Author_Table" ref="A1:J121" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D4467437-2A3E-4C21-932F-B15782EE29D5}" name="Author_Table" displayName="Author_Table" ref="A1:J121" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:J121" xr:uid="{758EA4D9-D01C-47C1-8B25-BCA71258E4C9}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3C78A6AF-5CC9-4ADB-9588-0AB44E80D9A8}" name="Repository_x000a_Rank" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{4B49AFD1-A12F-42DE-BB7E-A6178382257F}" name="Repository Name" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{B300A10E-70C1-45BD-8E60-576CD7063D52}" name="Marker" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{340F8572-4B5B-4C67-998E-C6BA34D5D977}" name="Trend in Mean" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{6AF3FF3A-19A1-4933-AB01-B6FD782A613E}" name="Author Eq (pre)" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{61FF835F-6F49-4A51-BDF2-EC9C724D2A68}" name="Author Eq (post)" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{77DB3632-DB2F-4911-80F1-A8AE918EA32D}" name="Change Direction_x000a_(Author Eq)" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{3C78A6AF-5CC9-4ADB-9588-0AB44E80D9A8}" name="Repository_x000a_Rank" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{4B49AFD1-A12F-42DE-BB7E-A6178382257F}" name="Repository Name" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{B300A10E-70C1-45BD-8E60-576CD7063D52}" name="Marker" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{340F8572-4B5B-4C67-998E-C6BA34D5D977}" name="Trend in Mean" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{6AF3FF3A-19A1-4933-AB01-B6FD782A613E}" name="Author Eq (pre)" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{61FF835F-6F49-4A51-BDF2-EC9C724D2A68}" name="Author Eq (post)" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{77DB3632-DB2F-4911-80F1-A8AE918EA32D}" name="Change Direction_x000a_(Author Eq)" dataDxfId="7">
       <calculatedColumnFormula>IF(Author_Table[Author Eq (pre)] &lt; Author_Table[Author Eq (post)], "Up", IF(Author_Table[Author Eq (pre)] &gt; Author_Table[Author Eq (post)], "Down", "No Change"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CDD643B7-34BC-4233-9956-24BDF133784F}" name="Author 80 (pre)" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{9C4A93B6-3443-43B0-AAE9-C2D727D9CA1D}" name="Author 80 (post)" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{F494A487-038B-4CB8-B0E5-3BB23E4F4BEF}" name="Change Direction_x000a_(Author 80)" dataDxfId="34">
+    <tableColumn id="5" xr3:uid="{CDD643B7-34BC-4233-9956-24BDF133784F}" name="Author 80 (pre)" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{9C4A93B6-3443-43B0-AAE9-C2D727D9CA1D}" name="Author 80 (post)" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{F494A487-038B-4CB8-B0E5-3BB23E4F4BEF}" name="Change Direction_x000a_(Author 80)" dataDxfId="4">
       <calculatedColumnFormula>IF(Author_Table[Author 80 (pre)] &lt; Author_Table[Author 80 (post)], "Up", IF(Author_Table[Author 80 (pre)] &gt; Author_Table[Author 80 (post)], "Down", "No Change"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2495,11 +2495,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{12F8B1DF-2997-4FD4-B471-3115399A6E5C}" name="Table5" displayName="Table5" ref="A1:B15" totalsRowShown="0" headerRowDxfId="30" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{12F8B1DF-2997-4FD4-B471-3115399A6E5C}" name="Table5" displayName="Table5" ref="A1:B15" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B15" xr:uid="{050D82F8-536D-4A38-9753-067603486D57}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F35B6690-83E7-4B46-8E7A-5C10EB645A1D}" name="Term" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{3F25AE98-D399-455C-8C4A-9E1B669EB79E}" name="Description" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{F35B6690-83E7-4B46-8E7A-5C10EB645A1D}" name="Term" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3F25AE98-D399-455C-8C4A-9E1B669EB79E}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7297,68 +7297,68 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="16" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="18" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="13" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="14" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="15" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="10" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="11" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="12" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G121">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="7" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="8" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="4" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="5" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="6" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J121">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7374,9 +7374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719927CC-3BAA-4815-83BA-36FB67172E3C}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11506,46 +11504,46 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J121">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"No Change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"Up"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>"Down"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>